<commit_message>
Our initial attempt to implement genetic algorithm into this task
</commit_message>
<xml_diff>
--- a/rule/fuzzy_rule.xlsx
+++ b/rule/fuzzy_rule.xlsx
@@ -1,34 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohameddhameemm/PycharmProjects/fuzzy-logic-project/rule/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2CA0786-806A-8442-9203-E56D4F8F703E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="16120" yWindow="2380" windowWidth="21580" windowHeight="10840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Impediment_Rule" sheetId="1" r:id="rId1"/>
-    <sheet name="Traffic_Light_Rule" sheetId="2" r:id="rId2"/>
-    <sheet name="fuzzy_values_initalize" sheetId="3" r:id="rId3"/>
-    <sheet name="fuzzy_values" sheetId="4" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Impediment_Rule" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Traffic_Light_Rule" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="fuzzy_values_initalize" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="fuzzy_values" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="44">
   <si>
     <t>Rule</t>
   </si>
@@ -84,6 +73,9 @@
     <t>Less_red</t>
   </si>
   <si>
+    <t>rule</t>
+  </si>
+  <si>
     <t>start</t>
   </si>
   <si>
@@ -93,16 +85,16 @@
     <t>step</t>
   </si>
   <si>
-    <t>rule</t>
+    <t>distance</t>
+  </si>
+  <si>
+    <t>angle</t>
   </si>
   <si>
     <t>light</t>
   </si>
   <si>
-    <t>distance</t>
-  </si>
-  <si>
-    <t>angle</t>
+    <t>speedo</t>
   </si>
   <si>
     <t>a</t>
@@ -145,9 +137,6 @@
   </si>
   <si>
     <t>light_greenred</t>
-  </si>
-  <si>
-    <t>speedo</t>
   </si>
   <si>
     <t>speedo_stop</t>
@@ -165,38 +154,28 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
+      <b val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -204,96 +183,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
+  <cellStyleXfs count="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="1">
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -593,19 +503,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.81640625" defaultRowHeight="12.5" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1025" width="11.5"/>
+    <col customWidth="1" max="1025" min="1" width="11.453125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -619,8 +533,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A2">
+    <row r="2" spans="1:4">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -633,8 +547,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3">
+    <row r="3" spans="1:4">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -647,8 +561,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4">
+    <row r="4" spans="1:4">
+      <c r="A4" t="n">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -661,8 +575,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5">
+    <row r="5" spans="1:4">
+      <c r="A5" t="n">
         <v>4</v>
       </c>
       <c r="B5" t="s">
@@ -675,8 +589,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6">
+    <row r="6" spans="1:4">
+      <c r="A6" t="n">
         <v>5</v>
       </c>
       <c r="B6" t="s">
@@ -689,8 +603,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7">
+    <row r="7" spans="1:4">
+      <c r="A7" t="n">
         <v>6</v>
       </c>
       <c r="B7" t="s">
@@ -703,8 +617,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8">
+    <row r="8" spans="1:4">
+      <c r="A8" t="n">
         <v>7</v>
       </c>
       <c r="B8" t="s">
@@ -717,8 +631,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9">
+    <row r="9" spans="1:4">
+      <c r="A9" t="n">
         <v>8</v>
       </c>
       <c r="B9" t="s">
@@ -731,8 +645,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A10">
+    <row r="10" spans="1:4">
+      <c r="A10" t="n">
         <v>9</v>
       </c>
       <c r="B10" t="s">
@@ -746,29 +660,37 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" paperSize="9" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
   </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.81640625" defaultRowHeight="12.5" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1025" width="11.5"/>
+    <col customWidth="1" max="1025" min="1" width="11.453125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -785,8 +707,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2">
+    <row r="2" spans="1:5">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -802,8 +724,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3">
+    <row r="3" spans="1:5">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -819,8 +741,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4">
+    <row r="4" spans="1:5">
+      <c r="A4" t="n">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -836,8 +758,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5">
+    <row r="5" spans="1:5">
+      <c r="A5" t="n">
         <v>4</v>
       </c>
       <c r="B5" t="s">
@@ -853,8 +775,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6">
+    <row r="6" spans="1:5">
+      <c r="A6" t="n">
         <v>5</v>
       </c>
       <c r="B6" t="s">
@@ -870,8 +792,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7">
+    <row r="7" spans="1:5">
+      <c r="A7" t="n">
         <v>6</v>
       </c>
       <c r="B7" t="s">
@@ -887,8 +809,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8">
+    <row r="8" spans="1:5">
+      <c r="A8" t="n">
         <v>7</v>
       </c>
       <c r="B8" t="s">
@@ -904,8 +826,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9">
+    <row r="9" spans="1:5">
+      <c r="A9" t="n">
         <v>8</v>
       </c>
       <c r="B9" t="s">
@@ -921,8 +843,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A10">
+    <row r="10" spans="1:5">
+      <c r="A10" t="n">
         <v>9</v>
       </c>
       <c r="B10" t="s">
@@ -938,8 +860,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A11">
+    <row r="11" spans="1:5">
+      <c r="A11" t="n">
         <v>10</v>
       </c>
       <c r="B11" t="s">
@@ -955,8 +877,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12">
+    <row r="12" spans="1:5">
+      <c r="A12" t="n">
         <v>11</v>
       </c>
       <c r="B12" t="s">
@@ -972,8 +894,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A13">
+    <row r="13" spans="1:5">
+      <c r="A13" t="n">
         <v>12</v>
       </c>
       <c r="B13" t="s">
@@ -989,8 +911,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A14">
+    <row r="14" spans="1:5">
+      <c r="A14" t="n">
         <v>13</v>
       </c>
       <c r="B14" t="s">
@@ -1006,8 +928,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A15">
+    <row r="15" spans="1:5">
+      <c r="A15" t="n">
         <v>14</v>
       </c>
       <c r="B15" t="s">
@@ -1023,8 +945,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A16">
+    <row r="16" spans="1:5">
+      <c r="A16" t="n">
         <v>15</v>
       </c>
       <c r="B16" t="s">
@@ -1040,8 +962,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A17">
+    <row r="17" spans="1:5">
+      <c r="A17" t="n">
         <v>16</v>
       </c>
       <c r="B17" t="s">
@@ -1057,8 +979,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A18">
+    <row r="18" spans="1:5">
+      <c r="A18" t="n">
         <v>17</v>
       </c>
       <c r="B18" t="s">
@@ -1074,8 +996,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A19">
+    <row r="19" spans="1:5">
+      <c r="A19" t="n">
         <v>18</v>
       </c>
       <c r="B19" t="s">
@@ -1091,8 +1013,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A20">
+    <row r="20" spans="1:5">
+      <c r="A20" t="n">
         <v>19</v>
       </c>
       <c r="B20" t="s">
@@ -1108,8 +1030,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A21">
+    <row r="21" spans="1:5">
+      <c r="A21" t="n">
         <v>20</v>
       </c>
       <c r="B21" t="s">
@@ -1125,8 +1047,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22">
+    <row r="22" spans="1:5">
+      <c r="A22" t="n">
         <v>21</v>
       </c>
       <c r="B22" t="s">
@@ -1142,8 +1064,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23">
+    <row r="23" spans="1:5">
+      <c r="A23" t="n">
         <v>22</v>
       </c>
       <c r="B23" t="s">
@@ -1159,8 +1081,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24">
+    <row r="24" spans="1:5">
+      <c r="A24" t="n">
         <v>23</v>
       </c>
       <c r="B24" t="s">
@@ -1176,8 +1098,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25">
+    <row r="25" spans="1:5">
+      <c r="A25" t="n">
         <v>24</v>
       </c>
       <c r="B25" t="s">
@@ -1193,8 +1115,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26">
+    <row r="26" spans="1:5">
+      <c r="A26" t="n">
         <v>25</v>
       </c>
       <c r="B26" t="s">
@@ -1210,8 +1132,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27">
+    <row r="27" spans="1:5">
+      <c r="A27" t="n">
         <v>26</v>
       </c>
       <c r="B27" t="s">
@@ -1227,8 +1149,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28">
+    <row r="28" spans="1:5">
+      <c r="A28" t="n">
         <v>27</v>
       </c>
       <c r="B28" t="s">
@@ -1244,8 +1166,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A29">
+    <row r="29" spans="1:5">
+      <c r="A29" t="n">
         <v>28</v>
       </c>
       <c r="B29" t="s">
@@ -1261,8 +1183,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A30">
+    <row r="30" spans="1:5">
+      <c r="A30" t="n">
         <v>29</v>
       </c>
       <c r="B30" t="s">
@@ -1278,8 +1200,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A31">
+    <row r="31" spans="1:5">
+      <c r="A31" t="n">
         <v>30</v>
       </c>
       <c r="B31" t="s">
@@ -1295,8 +1217,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A32">
+    <row r="32" spans="1:5">
+      <c r="A32" t="n">
         <v>31</v>
       </c>
       <c r="B32" t="s">
@@ -1312,8 +1234,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A33">
+    <row r="33" spans="1:5">
+      <c r="A33" t="n">
         <v>32</v>
       </c>
       <c r="B33" t="s">
@@ -1329,8 +1251,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A34">
+    <row r="34" spans="1:5">
+      <c r="A34" t="n">
         <v>33</v>
       </c>
       <c r="B34" t="s">
@@ -1346,8 +1268,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A35">
+    <row r="35" spans="1:5">
+      <c r="A35" t="n">
         <v>34</v>
       </c>
       <c r="B35" t="s">
@@ -1363,8 +1285,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A36">
+    <row r="36" spans="1:5">
+      <c r="A36" t="n">
         <v>35</v>
       </c>
       <c r="B36" t="s">
@@ -1380,8 +1302,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A37">
+    <row r="37" spans="1:5">
+      <c r="A37" t="n">
         <v>36</v>
       </c>
       <c r="B37" t="s">
@@ -1398,355 +1320,368 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" useFirstPageNumber="1" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
   </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D88F747-EEB0-4F43-96A2-DA7A287DCCCB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="10.90625" defaultRowHeight="12.5"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2010</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
         <v>23</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>2010</v>
-      </c>
-      <c r="D2">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>360</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
         <v>24</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>360</v>
-      </c>
-      <c r="D3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
         <v>21</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
+        <v>25</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
         <v>2</v>
       </c>
-      <c r="D5">
-        <v>1E-3</v>
+      <c r="D5" t="n">
+        <v>0.001</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B867DC7B-00A4-1C4E-846A-F4C15DA60C00}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>21.22087660622589</v>
+      </c>
+      <c r="E2" t="n">
+        <v>40.77350999270579</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="n">
+        <v>21.22087660622589</v>
+      </c>
+      <c r="C3" t="n">
+        <v>40.77350999270579</v>
+      </c>
+      <c r="D3" t="n">
+        <v>55.12040882872951</v>
+      </c>
+      <c r="E3" t="s"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="n">
+        <v>40.77350999270579</v>
+      </c>
+      <c r="C4" t="n">
+        <v>55.12040882872951</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2010</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>19.09909214338143</v>
+      </c>
+      <c r="E5" t="n">
+        <v>172.4861169495761</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="n">
+        <v>19.09909214338143</v>
+      </c>
+      <c r="C6" t="n">
+        <v>172.4861169495761</v>
+      </c>
+      <c r="D6" t="n">
+        <v>303.2045615654364</v>
+      </c>
+      <c r="E6" t="s"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="n">
+        <v>172.4861169495761</v>
+      </c>
+      <c r="C7" t="n">
+        <v>303.2045615654364</v>
+      </c>
+      <c r="D7" t="n">
+        <v>360</v>
+      </c>
+      <c r="E7" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>14.63775799082755</v>
+      </c>
+      <c r="D8" t="n">
         <v>21</v>
       </c>
-      <c r="B1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>70</v>
-      </c>
-      <c r="E2">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3">
-        <v>70</v>
-      </c>
-      <c r="C3">
-        <v>140</v>
-      </c>
-      <c r="D3">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4">
-        <v>140</v>
-      </c>
-      <c r="C4">
-        <v>210</v>
-      </c>
-      <c r="D4">
-        <v>2010</v>
-      </c>
-      <c r="E4">
-        <v>2010</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>7</v>
-      </c>
-      <c r="E5">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6">
-        <v>7</v>
-      </c>
-      <c r="C6">
-        <v>14</v>
-      </c>
-      <c r="D6">
+      <c r="E8" t="n">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7">
-        <v>10</v>
-      </c>
-      <c r="C7">
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>14.63775799082755</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="n">
+        <v>5.528606023584426</v>
+      </c>
+      <c r="C10" t="n">
+        <v>20.55553489405025</v>
+      </c>
+      <c r="D10" t="n">
         <v>21</v>
       </c>
-      <c r="D7">
-        <v>360</v>
-      </c>
-      <c r="E7">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="C8">
-        <v>6</v>
-      </c>
-      <c r="D8">
+      <c r="E10" t="n">
         <v>21</v>
       </c>
-      <c r="E8">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>3</v>
-      </c>
-      <c r="E9">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10">
-        <v>3</v>
-      </c>
-      <c r="C10">
-        <v>6</v>
-      </c>
-      <c r="D10">
-        <v>21</v>
-      </c>
-      <c r="E10">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>3</v>
-      </c>
-      <c r="E11">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+        <v>39</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>5.528606023584426</v>
+      </c>
+      <c r="E11" t="n">
+        <v>20.55553489405025</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>40</v>
       </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s"/>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>41</v>
       </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>0.5</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.1287602426791195</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.6167310409086104</v>
+      </c>
+      <c r="E13" t="s"/>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>42</v>
       </c>
-      <c r="B14">
-        <v>0.5</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B14" t="n">
+        <v>0.1287602426791195</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.6167310409086104</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1.839978562574001</v>
+      </c>
+      <c r="E14" t="s"/>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>43</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15">
-        <v>1.5</v>
-      </c>
-      <c r="D15">
+      <c r="B15" t="n">
+        <v>0.6167310409086104</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1.839978562574001</v>
+      </c>
+      <c r="D15" t="n">
         <v>2</v>
       </c>
-      <c r="E15">
+      <c r="E15" t="n">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixing beating the red light issue
</commit_message>
<xml_diff>
--- a/rule/fuzzy_rule.xlsx
+++ b/rule/fuzzy_rule.xlsx
@@ -663,8 +663,8 @@
   <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
   <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" paperSize="9" verticalDpi="300"/>
   <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
     <evenHeader/>
     <evenFooter/>
     <firstHeader/>
@@ -1323,8 +1323,8 @@
   <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
   <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" useFirstPageNumber="1" verticalDpi="300"/>
   <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
     <evenHeader/>
     <evenFooter/>
     <firstHeader/>
@@ -1464,10 +1464,10 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>21.22087660622589</v>
+        <v>15.5699101643917</v>
       </c>
       <c r="E2" t="n">
-        <v>40.77350999270579</v>
+        <v>145.1814757813382</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1475,13 +1475,13 @@
         <v>31</v>
       </c>
       <c r="B3" t="n">
-        <v>21.22087660622589</v>
+        <v>15.5699101643917</v>
       </c>
       <c r="C3" t="n">
-        <v>40.77350999270579</v>
+        <v>145.1814757813382</v>
       </c>
       <c r="D3" t="n">
-        <v>55.12040882872951</v>
+        <v>149.9585583888527</v>
       </c>
       <c r="E3" t="s"/>
     </row>
@@ -1490,10 +1490,10 @@
         <v>32</v>
       </c>
       <c r="B4" t="n">
-        <v>40.77350999270579</v>
+        <v>145.1814757813382</v>
       </c>
       <c r="C4" t="n">
-        <v>55.12040882872951</v>
+        <v>149.9585583888527</v>
       </c>
       <c r="D4" t="n">
         <v>2010</v>
@@ -1513,10 +1513,10 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>19.09909214338143</v>
+        <v>17.16511041311179</v>
       </c>
       <c r="E5" t="n">
-        <v>172.4861169495761</v>
+        <v>114.6172243513307</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1524,13 +1524,13 @@
         <v>34</v>
       </c>
       <c r="B6" t="n">
-        <v>19.09909214338143</v>
+        <v>17.16511041311179</v>
       </c>
       <c r="C6" t="n">
-        <v>172.4861169495761</v>
+        <v>114.6172243513307</v>
       </c>
       <c r="D6" t="n">
-        <v>303.2045615654364</v>
+        <v>201.6501654319696</v>
       </c>
       <c r="E6" t="s"/>
     </row>
@@ -1539,10 +1539,10 @@
         <v>35</v>
       </c>
       <c r="B7" t="n">
-        <v>172.4861169495761</v>
+        <v>114.6172243513307</v>
       </c>
       <c r="C7" t="n">
-        <v>303.2045615654364</v>
+        <v>201.6501654319696</v>
       </c>
       <c r="D7" t="n">
         <v>360</v>
@@ -1556,10 +1556,10 @@
         <v>36</v>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>1.499543122584523</v>
       </c>
       <c r="C8" t="n">
-        <v>14.63775799082755</v>
+        <v>20.37558392861101</v>
       </c>
       <c r="D8" t="n">
         <v>21</v>
@@ -1579,10 +1579,10 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>1.499543122584523</v>
       </c>
       <c r="E9" t="n">
-        <v>14.63775799082755</v>
+        <v>20.37558392861101</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1590,10 +1590,10 @@
         <v>38</v>
       </c>
       <c r="B10" t="n">
-        <v>5.528606023584426</v>
+        <v>10.56784383741841</v>
       </c>
       <c r="C10" t="n">
-        <v>20.55553489405025</v>
+        <v>18.40942901035632</v>
       </c>
       <c r="D10" t="n">
         <v>21</v>
@@ -1613,10 +1613,10 @@
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>5.528606023584426</v>
+        <v>10.56784383741841</v>
       </c>
       <c r="E11" t="n">
-        <v>20.55553489405025</v>
+        <v>18.40942901035632</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1642,10 +1642,10 @@
         <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>0.1287602426791195</v>
+        <v>0.2961582525032522</v>
       </c>
       <c r="D13" t="n">
-        <v>0.6167310409086104</v>
+        <v>0.875326724110622</v>
       </c>
       <c r="E13" t="s"/>
     </row>
@@ -1654,13 +1654,13 @@
         <v>42</v>
       </c>
       <c r="B14" t="n">
-        <v>0.1287602426791195</v>
+        <v>0.2961582525032522</v>
       </c>
       <c r="C14" t="n">
-        <v>0.6167310409086104</v>
+        <v>0.875326724110622</v>
       </c>
       <c r="D14" t="n">
-        <v>1.839978562574001</v>
+        <v>1.851474461442805</v>
       </c>
       <c r="E14" t="s"/>
     </row>
@@ -1669,10 +1669,10 @@
         <v>43</v>
       </c>
       <c r="B15" t="n">
-        <v>0.6167310409086104</v>
+        <v>0.875326724110622</v>
       </c>
       <c r="C15" t="n">
-        <v>1.839978562574001</v>
+        <v>1.851474461442805</v>
       </c>
       <c r="D15" t="n">
         <v>2</v>

</xml_diff>